<commit_message>
add round 3 data files
</commit_message>
<xml_diff>
--- a/作品总计.xlsx
+++ b/作品总计.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/fqx/Dropbox/天坑企划/拉力赛/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/fqx/Dropbox/LLS3/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{AC2460F4-78AD-8247-8C23-924F6612EA4D}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D7B2540B-3776-784D-BC36-4CD7B985E4F0}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16000" xr2:uid="{21474D36-4D57-C348-AD7E-A6C14114E78A}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="15540" xr2:uid="{21474D36-4D57-C348-AD7E-A6C14114E78A}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -491,7 +491,7 @@
   <dimension ref="A1:F12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -646,6 +646,15 @@
       <c r="C8" t="s">
         <v>10</v>
       </c>
+      <c r="D8">
+        <v>1546</v>
+      </c>
+      <c r="E8">
+        <v>369</v>
+      </c>
+      <c r="F8">
+        <v>3238</v>
+      </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9">

</xml_diff>